<commit_message>
fix: Refine data wrangling and Univariate Analysis
The features chosen for analysis are changed in order to match the
requirements of the analysis.
</commit_message>
<xml_diff>
--- a/Prosper Loan Data - Variable Definitions.xlsx
+++ b/Prosper Loan Data - Variable Definitions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Data Analysis\Data Visualization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Data Analysis\Data Visualisation\loan-data-visualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEB4AAB-6B13-4FB5-9687-D24E624279B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A22A05-0FB0-4336-B927-696FA2C35252}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -581,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -613,6 +613,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -935,8 +938,8 @@
   <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -963,7 +966,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1011,7 +1014,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1019,7 +1022,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1067,7 +1070,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -1075,7 +1078,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -1083,7 +1086,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -1091,7 +1094,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -1099,7 +1102,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -1115,7 +1118,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -1155,7 +1158,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -1163,7 +1166,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -1331,7 +1334,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="6" t="s">
         <v>96</v>
       </c>
       <c r="B49" s="7" t="s">
@@ -1347,7 +1350,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="8" t="s">
         <v>100</v>
       </c>
       <c r="B51" s="7" t="s">
@@ -1363,7 +1366,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="9" t="s">
         <v>104</v>
       </c>
       <c r="B53" s="7" t="s">
@@ -1371,7 +1374,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="9" t="s">
         <v>106</v>
       </c>
       <c r="B54" s="7" t="s">
@@ -1379,7 +1382,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="9" t="s">
         <v>108</v>
       </c>
       <c r="B55" s="7" t="s">
@@ -1467,7 +1470,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="8" t="s">
+      <c r="A66" s="6" t="s">
         <v>130</v>
       </c>
       <c r="B66" s="7" t="s">
@@ -1475,7 +1478,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
+      <c r="A67" s="8" t="s">
         <v>132</v>
       </c>
       <c r="B67" s="7" t="s">
@@ -1571,7 +1574,7 @@
       </c>
     </row>
     <row r="79" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="8" t="s">
+      <c r="A79" s="6" t="s">
         <v>156</v>
       </c>
       <c r="B79" s="7" t="s">

</xml_diff>